<commit_message>
Update all benchmarking files to include data about which compiled code it is running on, and which dataset. Also made some changes to benchmarking results in Excel. And made new file with cengine with a buffered reader
</commit_message>
<xml_diff>
--- a/benchmarking/results_of_count_function.xlsx
+++ b/benchmarking/results_of_count_function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejer/Desktop/rustengine/benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01295C-BC25-F341-B259-D9828503E9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED72B80C-5C9E-9C4B-81E5-4B98D38CC99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28240" windowHeight="16300" firstSheet="2" activeTab="7" xr2:uid="{E7C49614-21E1-0C49-99A7-E55A94F1DDD0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28240" windowHeight="16300" xr2:uid="{E7C49614-21E1-0C49-99A7-E55A94F1DDD0}"/>
   </bookViews>
   <sheets>
     <sheet name="results_C" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,13 @@
     <sheet name="results_rust_tiny_vs_large" sheetId="6" r:id="rId5"/>
     <sheet name="results_c_tiny_vs_large" sheetId="7" r:id="rId6"/>
     <sheet name="results_rust_with_file" sheetId="8" r:id="rId7"/>
-    <sheet name="results_rust_buffered_file_read" sheetId="9" r:id="rId8"/>
-    <sheet name="results_c_with_new _count" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="49">
   <si>
     <t>timestamp</t>
   </si>
@@ -156,13 +154,25 @@
     <t>0.13</t>
   </si>
   <si>
-    <t>0.11</t>
+    <t>this is run on the first cengine, but compiled with different flags, to see if it got faster</t>
   </si>
   <si>
-    <t>enwiki-tiny</t>
+    <t>This is run on rustengine_1point1</t>
   </si>
   <si>
-    <t>enwiki-large</t>
+    <t>this is run with rustengine</t>
+  </si>
+  <si>
+    <t>This is run with rustengine_1point1</t>
+  </si>
+  <si>
+    <t>this is run with cengine</t>
+  </si>
+  <si>
+    <t>this is run with a deleted directory, but it was code from chat about how to use file</t>
+  </si>
+  <si>
+    <t>This is run on the first cengine - compiled it is called scanner</t>
   </si>
 </sst>
 </file>
@@ -9445,10 +9455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4542A0EE-E810-2E4F-85C5-641725D84E0B}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9730,6 +9740,11 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -9738,10 +9753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AC3A7D-AD6B-D745-98B0-2F8C85FAB609}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9994,6 +10009,11 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -10002,10 +10022,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F661AC2D-B4A7-C34C-9745-B1559BD3183F}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10258,6 +10278,11 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -10266,10 +10291,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF4EC68-ED40-814B-8139-7A0896210DB8}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10522,6 +10547,11 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -10530,10 +10560,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4597B490-6C92-5D4B-AFCD-53A70876BC7A}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10652,6 +10682,11 @@
         <v>39</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -10659,10 +10694,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BB982F-7448-F448-B1D0-FABAEBB49C80}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10776,6 +10811,11 @@
       </c>
       <c r="L3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -10785,10 +10825,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25AA84E-1CCB-884C-AD6B-117BB5DD5FEF}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10898,256 +10938,9 @@
         <v>1</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E6CEC5-4820-7343-BF49-0EA8C218AC26}">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>45560.614340277774</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="F2">
-        <v>588</v>
-      </c>
-      <c r="G2">
-        <v>28</v>
-      </c>
-      <c r="H2">
-        <v>314</v>
-      </c>
-      <c r="I2">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>45560.614432870374</v>
-      </c>
-      <c r="B3" s="4">
-        <v>5.88</v>
-      </c>
-      <c r="C3" s="4">
-        <v>5.76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.99</v>
-      </c>
-      <c r="F3">
-        <v>668</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>364</v>
-      </c>
-      <c r="I3">
-        <v>790</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D83573-2F4D-0544-BAB6-C55913144051}">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>45560.631863425922</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="F2">
-        <v>476</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>312</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>45560.631921296299</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="C3" s="4">
-        <v>3.99</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="F3">
-        <v>476</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>310</v>
-      </c>
-      <c r="I3">
-        <v>1840</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>